<commit_message>
BCOP-1943 Updating CNN Inventory
git-tfs-id: [http://devvm01tfs03.telamericamedia.com:8080/tfs/CMWPA]$/Telamerica/Broadcast/OnDeck;C21448
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/CNNAMPMBarterObligations_Clean.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/CNNAMPMBarterObligations_Clean.xlsx
@@ -1015,9 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1215,7 +1213,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H5" s="25">
         <v>1</v>

</xml_diff>